<commit_message>
add role and power
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
   <si>
     <t>user</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -47,6 +47,42 @@
   </si>
   <si>
     <t>tablename</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>role</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userrole</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>roleid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rolepower</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>powerid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>power</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -391,55 +427,125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="B4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="B5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="B6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="B7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="B8" t="s">
         <v>5</v>
       </c>

</xml_diff>